<commit_message>
css edited and scrum updated
</commit_message>
<xml_diff>
--- a/ScrumProjectKesa.xlsx
+++ b/ScrumProjectKesa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c0ec9f24d8d72cc2/OmatAsiat/GitHubRepos/ProjectKesa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="325" documentId="13_ncr:1_{EBFB5D00-5B16-4383-ADE2-85B692247430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{916E37EF-4F73-40AF-907D-60C6F3A2CB3E}"/>
+  <xr:revisionPtr revIDLastSave="326" documentId="13_ncr:1_{EBFB5D00-5B16-4383-ADE2-85B692247430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CEE5F561-2DA5-4B33-A527-6F6E7D19E49B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="835" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="28065" windowHeight="15735" tabRatio="835" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guide" sheetId="7" r:id="rId1"/>
@@ -4586,7 +4586,7 @@
   <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4874,7 +4874,7 @@
       <c r="B11" s="47"/>
       <c r="C11" s="47"/>
       <c r="D11" s="47" t="s">
-        <v>105</v>
+        <v>43</v>
       </c>
       <c r="E11" s="47"/>
       <c r="F11" s="47"/>

</xml_diff>

<commit_message>
Scrum updated. A successful message when sign is successful added with html css and js
</commit_message>
<xml_diff>
--- a/ScrumProjectKesa.xlsx
+++ b/ScrumProjectKesa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c0ec9f24d8d72cc2/OmatAsiat/GitHubRepos/ProjectKesa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="411" documentId="13_ncr:1_{EBFB5D00-5B16-4383-ADE2-85B692247430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4610B9A-FF64-4903-8250-4555BFE9BB66}"/>
+  <xr:revisionPtr revIDLastSave="422" documentId="13_ncr:1_{EBFB5D00-5B16-4383-ADE2-85B692247430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68D3A224-4CE4-4671-8EF0-E076B5C49484}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="835" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="120">
   <si>
     <t>Content</t>
   </si>
@@ -329,15 +329,9 @@
     <t xml:space="preserve">Connect to users db table and delete the profile basedon the ID </t>
   </si>
   <si>
-    <t xml:space="preserve">Sprint Backlog : Sprint 1 22.06.22- </t>
-  </si>
-  <si>
     <t xml:space="preserve">Sprint Backlog : Sprint 3 </t>
   </si>
   <si>
-    <t xml:space="preserve">Sprint Backlog : Sprint 2 </t>
-  </si>
-  <si>
     <t xml:space="preserve">User Story #1:  As a user, I am able to register and become a registerd user. </t>
   </si>
   <si>
@@ -396,6 +390,15 @@
   </si>
   <si>
     <t>Create a doa function to check for duplicate emails and return an error message for the user</t>
+  </si>
+  <si>
+    <t>Sprint Backlog : Sprint 1 22.06.22- 03.08.22</t>
+  </si>
+  <si>
+    <t>Sprint Backlog : Sprint 2 03.08.22-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a function to show the a message once sign up is completed on main page. </t>
   </si>
 </sst>
 </file>
@@ -4622,7 +4625,7 @@
   <dimension ref="A1:S42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4635,7 +4638,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="80" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="B1" s="81"/>
       <c r="C1" s="81"/>
@@ -4724,7 +4727,7 @@
     </row>
     <row r="4" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="61" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B4" s="45"/>
       <c r="C4" s="36" t="s">
@@ -4780,7 +4783,7 @@
     </row>
     <row r="6" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="60" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B6" s="48"/>
       <c r="C6" s="49"/>
@@ -4805,7 +4808,7 @@
     </row>
     <row r="7" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="60" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B7" s="48"/>
       <c r="C7" s="49"/>
@@ -4830,7 +4833,7 @@
     </row>
     <row r="8" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="60" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B8" s="47"/>
       <c r="C8" s="49"/>
@@ -4897,7 +4900,7 @@
     </row>
     <row r="11" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B11" s="37">
         <v>2</v>
@@ -4924,7 +4927,7 @@
     </row>
     <row r="12" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B12" s="47"/>
       <c r="C12" s="51"/>
@@ -4949,7 +4952,7 @@
     </row>
     <row r="13" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="47" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B13" s="47"/>
       <c r="C13" s="51"/>
@@ -4974,7 +4977,7 @@
     </row>
     <row r="14" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="47" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B14" s="47"/>
       <c r="C14" s="51"/>
@@ -4999,7 +5002,7 @@
     </row>
     <row r="15" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="47" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B15" s="47"/>
       <c r="C15" s="51"/>
@@ -5024,7 +5027,7 @@
     </row>
     <row r="16" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="47" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B16" s="47"/>
       <c r="C16" s="51"/>
@@ -5049,7 +5052,7 @@
     </row>
     <row r="17" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="58" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B17" s="47"/>
       <c r="C17" s="49"/>
@@ -5074,7 +5077,7 @@
     </row>
     <row r="18" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="50" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B18" s="37">
         <v>4</v>
@@ -5083,7 +5086,7 @@
         <v>27</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E18" s="46"/>
       <c r="F18" s="46"/>
@@ -5103,7 +5106,7 @@
     </row>
     <row r="19" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="60" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B19" s="47"/>
       <c r="C19" s="47"/>
@@ -5128,7 +5131,7 @@
     </row>
     <row r="20" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="60" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B20" s="47"/>
       <c r="C20" s="47"/>
@@ -5153,7 +5156,7 @@
     </row>
     <row r="21" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="60" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B21" s="47"/>
       <c r="C21" s="47"/>
@@ -5178,7 +5181,7 @@
     </row>
     <row r="22" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="58" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B22" s="47"/>
       <c r="C22" s="47"/>
@@ -5203,7 +5206,7 @@
     </row>
     <row r="23" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="58" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B23" s="47"/>
       <c r="C23" s="47"/>
@@ -5227,10 +5230,14 @@
       <c r="S23" s="39"/>
     </row>
     <row r="24" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="58"/>
+      <c r="A24" s="58" t="s">
+        <v>119</v>
+      </c>
       <c r="B24" s="47"/>
       <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
+      <c r="D24" s="47" t="s">
+        <v>43</v>
+      </c>
       <c r="E24" s="47"/>
       <c r="F24" s="47"/>
       <c r="G24" s="47"/>
@@ -5249,7 +5256,7 @@
     </row>
     <row r="25" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="50" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B25" s="37">
         <v>6</v>
@@ -5258,7 +5265,7 @@
         <v>27</v>
       </c>
       <c r="D25" s="37" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E25" s="46"/>
       <c r="F25" s="46"/>
@@ -5362,7 +5369,7 @@
     </row>
     <row r="30" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="37" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B30" s="37">
         <v>4</v>
@@ -5371,7 +5378,7 @@
         <v>27</v>
       </c>
       <c r="D30" s="37" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E30" s="46"/>
       <c r="F30" s="46"/>
@@ -5686,7 +5693,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="82" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="B1" s="83"/>
       <c r="C1" s="83"/>
@@ -5747,9 +5754,15 @@
       <c r="S2" s="14"/>
     </row>
     <row r="3" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="12"/>
+      <c r="A3" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="11">
+        <v>6</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
@@ -5994,9 +6007,15 @@
       <c r="S14" s="14"/>
     </row>
     <row r="15" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
+      <c r="A15" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="11">
+        <v>4</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
@@ -6560,7 +6579,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="82" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="83"/>
       <c r="C1" s="83"/>

</xml_diff>

<commit_message>
'Profile' page creatd, but only the navbar that sticks when scrollingdownthe page is created. Logo added to open tabs. Scrum updated
</commit_message>
<xml_diff>
--- a/ScrumProjectKesa.xlsx
+++ b/ScrumProjectKesa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c0ec9f24d8d72cc2/OmatAsiat/GitHubRepos/ProjectKesa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="422" documentId="13_ncr:1_{EBFB5D00-5B16-4383-ADE2-85B692247430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68D3A224-4CE4-4671-8EF0-E076B5C49484}"/>
+  <xr:revisionPtr revIDLastSave="434" documentId="13_ncr:1_{EBFB5D00-5B16-4383-ADE2-85B692247430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A362D297-7207-4CA9-8FA6-18AFF22AB90A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="835" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="835" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guide" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="122">
   <si>
     <t>Content</t>
   </si>
@@ -134,9 +134,6 @@
     <t>X</t>
   </si>
   <si>
-    <t xml:space="preserve">Date: 4.4.2022 </t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -399,6 +396,15 @@
   </si>
   <si>
     <t xml:space="preserve">Create a function to show the a message once sign up is completed on main page. </t>
+  </si>
+  <si>
+    <t>Create a profile page for users to land on after sgining in using jsp, html, css nad js</t>
+  </si>
+  <si>
+    <t>Navbar on the page sticks while scroling using window.onscroll function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date: 3.8.2022 </t>
   </si>
 </sst>
 </file>
@@ -3389,7 +3395,7 @@
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
       <c r="D2" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E2" s="31"/>
       <c r="F2" s="31"/>
@@ -3398,7 +3404,7 @@
     </row>
     <row r="3" spans="2:8" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B3" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -3409,7 +3415,7 @@
     </row>
     <row r="4" spans="2:8" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B4" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -3530,7 +3536,7 @@
     </row>
     <row r="4" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="2">
         <v>6</v>
@@ -3541,7 +3547,7 @@
     </row>
     <row r="5" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="2">
         <v>6</v>
@@ -3552,7 +3558,7 @@
     </row>
     <row r="6" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="2">
         <v>6</v>
@@ -3563,7 +3569,7 @@
     </row>
     <row r="7" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="2">
         <v>4</v>
@@ -3574,7 +3580,7 @@
     </row>
     <row r="8" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="2">
         <v>6</v>
@@ -3585,7 +3591,7 @@
     </row>
     <row r="9" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="2">
         <v>2</v>
@@ -3596,7 +3602,7 @@
     </row>
     <row r="10" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="2">
         <v>4</v>
@@ -3607,7 +3613,7 @@
     </row>
     <row r="11" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="2">
         <v>4</v>
@@ -3618,7 +3624,7 @@
     </row>
     <row r="12" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" s="2">
         <v>4</v>
@@ -3629,7 +3635,7 @@
     </row>
     <row r="13" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" s="2">
         <v>4</v>
@@ -3640,7 +3646,7 @@
     </row>
     <row r="14" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B14" s="2">
         <v>2</v>
@@ -3911,7 +3917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62CD205-9E86-46AF-9920-145C3DB823CA}">
   <dimension ref="C1:M64"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
@@ -3940,10 +3946,10 @@
         <v>17</v>
       </c>
       <c r="E3" s="67" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="77" t="s">
         <v>74</v>
-      </c>
-      <c r="H3" s="77" t="s">
-        <v>75</v>
       </c>
       <c r="I3" s="77"/>
       <c r="J3" s="77"/>
@@ -3956,12 +3962,12 @@
       <c r="D4" s="32"/>
       <c r="E4" s="16"/>
       <c r="H4" s="78" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I4" s="78"/>
       <c r="J4" s="78"/>
       <c r="K4" s="79" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L4" s="79"/>
       <c r="M4" s="79"/>
@@ -3979,7 +3985,7 @@
     </row>
     <row r="6" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="16"/>
@@ -4037,7 +4043,7 @@
     <row r="11" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="33"/>
       <c r="D11" s="33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E11" s="69"/>
       <c r="H11" s="78"/>
@@ -4091,7 +4097,7 @@
       <c r="D15" s="35"/>
       <c r="E15" s="35"/>
       <c r="I15" s="74" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J15" s="75"/>
       <c r="K15" s="75"/>
@@ -4110,7 +4116,7 @@
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C17" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" s="34" t="s">
         <v>21</v>
@@ -4149,13 +4155,13 @@
     <row r="21" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C21" s="32"/>
       <c r="D21" s="32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E21" s="68"/>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C22" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D22" s="32" t="s">
         <v>23</v>
@@ -4176,13 +4182,13 @@
     <row r="25" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C25" s="34"/>
       <c r="D25" s="34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E25" s="68"/>
     </row>
     <row r="26" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C26" s="34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D26" s="34" t="s">
         <v>23</v>
@@ -4202,20 +4208,20 @@
     <row r="29" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C29" s="33"/>
       <c r="D29" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E29" s="16"/>
     </row>
     <row r="30" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C30" s="33"/>
       <c r="D30" s="33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E30" s="16"/>
     </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C31" s="33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D31" s="33"/>
       <c r="E31" s="16"/>
@@ -4233,16 +4239,16 @@
     <row r="34" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C34" s="34"/>
       <c r="D34" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E34" s="16"/>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C35" s="34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D35" s="34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E35" s="16"/>
     </row>
@@ -4265,7 +4271,7 @@
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C39" s="32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D39" s="32"/>
       <c r="E39" s="68"/>
@@ -4283,23 +4289,23 @@
     <row r="42" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C42" s="33"/>
       <c r="D42" s="33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E42" s="68"/>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C43" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D43" s="33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E43" s="68"/>
     </row>
     <row r="44" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C44" s="33"/>
       <c r="D44" s="33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E44" s="68"/>
     </row>
@@ -4311,30 +4317,30 @@
     <row r="46" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C46" s="34"/>
       <c r="D46" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E46" s="16"/>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C47" s="34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D47" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E47" s="16"/>
     </row>
     <row r="48" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C48" s="34"/>
       <c r="D48" s="34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E48" s="16"/>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C49" s="34"/>
       <c r="D49" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E49" s="16"/>
     </row>
@@ -4346,13 +4352,13 @@
     <row r="51" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C51" s="32"/>
       <c r="D51" s="32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E51" s="68"/>
     </row>
     <row r="52" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C52" s="32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D52" s="32"/>
       <c r="E52" s="68"/>
@@ -4370,13 +4376,13 @@
     <row r="55" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C55" s="33"/>
       <c r="D55" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E55" s="68"/>
     </row>
     <row r="56" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C56" s="33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D56" s="33"/>
       <c r="E56" s="68"/>
@@ -4394,20 +4400,20 @@
     <row r="59" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C59" s="34"/>
       <c r="D59" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E59" s="68"/>
     </row>
     <row r="60" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C60" s="34"/>
       <c r="D60" s="34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E60" s="68"/>
     </row>
     <row r="61" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C61" s="34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D61" s="34"/>
       <c r="E61" s="68"/>
@@ -4448,7 +4454,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4470,16 +4476,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="27" t="s">
         <v>65</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -4497,7 +4503,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -4505,7 +4511,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -4515,13 +4521,15 @@
       <c r="A6" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="C6" s="1"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>31</v>
+        <v>121</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4529,7 +4537,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -4545,7 +4553,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -4553,7 +4561,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -4569,7 +4577,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -4577,7 +4585,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -4593,7 +4601,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -4624,8 +4632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE6088DA-74CF-4F3C-ACDE-C67EABB84574}">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4638,7 +4646,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="80" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B1" s="81"/>
       <c r="C1" s="81"/>
@@ -4661,31 +4669,31 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="C2" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="D2" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="E2" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="F2" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="43" t="s">
+      <c r="G2" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="43" t="s">
+      <c r="H2" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="43" t="s">
+      <c r="I2" s="43" t="s">
         <v>40</v>
-      </c>
-      <c r="I2" s="43" t="s">
-        <v>41</v>
       </c>
       <c r="J2" s="39"/>
       <c r="K2" s="39"/>
@@ -4700,14 +4708,12 @@
     </row>
     <row r="3" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="61" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="45"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36" t="s">
         <v>42</v>
-      </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="36" t="s">
-        <v>43</v>
       </c>
       <c r="E3" s="45"/>
       <c r="F3" s="45"/>
@@ -4727,14 +4733,12 @@
     </row>
     <row r="4" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="61" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" s="45"/>
-      <c r="C4" s="36" t="s">
-        <v>27</v>
-      </c>
+      <c r="C4" s="36"/>
       <c r="D4" s="36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" s="45"/>
       <c r="F4" s="45"/>
@@ -4754,16 +4758,14 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="37">
         <v>3</v>
       </c>
-      <c r="C5" s="37" t="s">
-        <v>27</v>
-      </c>
+      <c r="C5" s="37"/>
       <c r="D5" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" s="46"/>
       <c r="F5" s="46"/>
@@ -4783,12 +4785,12 @@
     </row>
     <row r="6" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="60" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="48"/>
       <c r="C6" s="49"/>
       <c r="D6" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="47"/>
       <c r="F6" s="47"/>
@@ -4808,12 +4810,12 @@
     </row>
     <row r="7" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="60" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B7" s="48"/>
       <c r="C7" s="49"/>
       <c r="D7" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" s="47"/>
       <c r="F7" s="47"/>
@@ -4833,12 +4835,12 @@
     </row>
     <row r="8" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="60" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B8" s="47"/>
       <c r="C8" s="49"/>
       <c r="D8" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E8" s="47"/>
       <c r="F8" s="47"/>
@@ -4900,14 +4902,14 @@
     </row>
     <row r="11" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B11" s="37">
         <v>2</v>
       </c>
       <c r="C11" s="46"/>
       <c r="D11" s="46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" s="46"/>
       <c r="F11" s="46"/>
@@ -4927,12 +4929,12 @@
     </row>
     <row r="12" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B12" s="47"/>
       <c r="C12" s="51"/>
       <c r="D12" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E12" s="47"/>
       <c r="F12" s="47"/>
@@ -4952,12 +4954,12 @@
     </row>
     <row r="13" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B13" s="47"/>
       <c r="C13" s="51"/>
       <c r="D13" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E13" s="47"/>
       <c r="F13" s="47"/>
@@ -4977,12 +4979,12 @@
     </row>
     <row r="14" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="47" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B14" s="47"/>
       <c r="C14" s="51"/>
       <c r="D14" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="47"/>
       <c r="F14" s="47"/>
@@ -5002,12 +5004,12 @@
     </row>
     <row r="15" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="47" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B15" s="47"/>
       <c r="C15" s="51"/>
       <c r="D15" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E15" s="47"/>
       <c r="F15" s="47"/>
@@ -5027,12 +5029,12 @@
     </row>
     <row r="16" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="47" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B16" s="47"/>
       <c r="C16" s="51"/>
       <c r="D16" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E16" s="47"/>
       <c r="F16" s="47"/>
@@ -5052,12 +5054,12 @@
     </row>
     <row r="17" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B17" s="47"/>
       <c r="C17" s="49"/>
       <c r="D17" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E17" s="47"/>
       <c r="F17" s="47"/>
@@ -5077,16 +5079,14 @@
     </row>
     <row r="18" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="50" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B18" s="37">
         <v>4</v>
       </c>
-      <c r="C18" s="37" t="s">
-        <v>27</v>
-      </c>
+      <c r="C18" s="37"/>
       <c r="D18" s="37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E18" s="46"/>
       <c r="F18" s="46"/>
@@ -5106,12 +5106,12 @@
     </row>
     <row r="19" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="60" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B19" s="47"/>
       <c r="C19" s="47"/>
       <c r="D19" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E19" s="47"/>
       <c r="F19" s="47"/>
@@ -5131,12 +5131,12 @@
     </row>
     <row r="20" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="60" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B20" s="47"/>
       <c r="C20" s="47"/>
       <c r="D20" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E20" s="47"/>
       <c r="F20" s="47"/>
@@ -5156,12 +5156,12 @@
     </row>
     <row r="21" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="60" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B21" s="47"/>
       <c r="C21" s="47"/>
       <c r="D21" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E21" s="47"/>
       <c r="F21" s="47"/>
@@ -5181,12 +5181,12 @@
     </row>
     <row r="22" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="58" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B22" s="47"/>
       <c r="C22" s="47"/>
       <c r="D22" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E22" s="47"/>
       <c r="F22" s="47"/>
@@ -5206,12 +5206,12 @@
     </row>
     <row r="23" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="58" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B23" s="47"/>
       <c r="C23" s="47"/>
       <c r="D23" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E23" s="47"/>
       <c r="F23" s="47"/>
@@ -5231,12 +5231,12 @@
     </row>
     <row r="24" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="58" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B24" s="47"/>
       <c r="C24" s="47"/>
       <c r="D24" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E24" s="47"/>
       <c r="F24" s="47"/>
@@ -5256,16 +5256,14 @@
     </row>
     <row r="25" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="50" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B25" s="37">
         <v>6</v>
       </c>
-      <c r="C25" s="37" t="s">
-        <v>27</v>
-      </c>
+      <c r="C25" s="37"/>
       <c r="D25" s="37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E25" s="46"/>
       <c r="F25" s="46"/>
@@ -5369,16 +5367,14 @@
     </row>
     <row r="30" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B30" s="37">
         <v>4</v>
       </c>
-      <c r="C30" s="37" t="s">
-        <v>27</v>
-      </c>
+      <c r="C30" s="37"/>
       <c r="D30" s="37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E30" s="46"/>
       <c r="F30" s="46"/>
@@ -5629,7 +5625,7 @@
     </row>
     <row r="42" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="54" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B42" s="54">
         <f>SUM(B3:B41)</f>
@@ -5681,8 +5677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B586DF3-05CE-45CD-BBBF-F44EAB136942}">
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:S1"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5693,7 +5689,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="82" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B1" s="83"/>
       <c r="C1" s="83"/>
@@ -5716,31 +5712,31 @@
     </row>
     <row r="2" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>36</v>
-      </c>
       <c r="E2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="I2" s="10" t="s">
         <v>48</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>49</v>
       </c>
       <c r="J2" s="14"/>
       <c r="K2" s="14"/>
@@ -5755,14 +5751,12 @@
     </row>
     <row r="3" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" s="11">
         <v>6</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>27</v>
-      </c>
+      <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
@@ -5781,7 +5775,9 @@
       <c r="S3" s="14"/>
     </row>
     <row r="4" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="62"/>
+      <c r="A4" s="62" t="s">
+        <v>119</v>
+      </c>
       <c r="B4" s="13"/>
       <c r="C4" s="47"/>
       <c r="D4" s="47"/>
@@ -5802,7 +5798,9 @@
       <c r="S4" s="14"/>
     </row>
     <row r="5" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="63"/>
+      <c r="A5" s="63" t="s">
+        <v>120</v>
+      </c>
       <c r="B5" s="13"/>
       <c r="C5" s="47"/>
       <c r="D5" s="47"/>
@@ -6008,14 +6006,12 @@
     </row>
     <row r="15" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B15" s="11">
         <v>4</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>27</v>
-      </c>
+      <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
@@ -6518,7 +6514,7 @@
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -6579,7 +6575,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="82" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" s="83"/>
       <c r="C1" s="83"/>
@@ -6602,31 +6598,31 @@
     </row>
     <row r="2" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>36</v>
-      </c>
       <c r="E2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="I2" s="10" t="s">
         <v>48</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>49</v>
       </c>
       <c r="J2" s="14"/>
       <c r="K2" s="14"/>
@@ -7390,7 +7386,7 @@
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>

</xml_diff>

<commit_message>
Login servlet created uses post method, Logout servlet creatred, A servlet to show user info created, updates to profile.jsp
</commit_message>
<xml_diff>
--- a/ScrumProjectKesa.xlsx
+++ b/ScrumProjectKesa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c0ec9f24d8d72cc2/OmatAsiat/GitHubRepos/ProjectKesa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="435" documentId="13_ncr:1_{EBFB5D00-5B16-4383-ADE2-85B692247430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{533BEEC8-63BE-4D09-91A0-594C71B94EB6}"/>
+  <xr:revisionPtr revIDLastSave="439" documentId="13_ncr:1_{EBFB5D00-5B16-4383-ADE2-85B692247430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C1612C6-4607-47D1-B43B-FCBA3C77ED8D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="835" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,6 +23,7 @@
     <sheet name="sprint_backlog_sprint3" sheetId="17" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="125">
   <si>
     <t>Content</t>
   </si>
@@ -405,6 +406,15 @@
   </si>
   <si>
     <t>Navbar on the page sticks while scroling using window.onscroll function.</t>
+  </si>
+  <si>
+    <t>Logout servlet creatred</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A servlet to show user info created </t>
+  </si>
+  <si>
+    <t>Login servlet created uses post method</t>
   </si>
 </sst>
 </file>
@@ -3917,7 +3927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62CD205-9E86-46AF-9920-145C3DB823CA}">
   <dimension ref="C1:M64"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
@@ -5678,7 +5688,7 @@
   <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5821,7 +5831,9 @@
       <c r="S5" s="14"/>
     </row>
     <row r="6" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="64"/>
+      <c r="A6" s="64" t="s">
+        <v>124</v>
+      </c>
       <c r="B6" s="13"/>
       <c r="C6" s="47"/>
       <c r="D6" s="47"/>
@@ -5842,7 +5854,9 @@
       <c r="S6" s="14"/>
     </row>
     <row r="7" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="63"/>
+      <c r="A7" s="63" t="s">
+        <v>122</v>
+      </c>
       <c r="B7" s="13"/>
       <c r="C7" s="47"/>
       <c r="D7" s="47"/>
@@ -5863,7 +5877,9 @@
       <c r="S7" s="14"/>
     </row>
     <row r="8" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="61"/>
+      <c r="A8" s="61" t="s">
+        <v>123</v>
+      </c>
       <c r="C8" s="49"/>
       <c r="D8" s="49"/>
       <c r="I8" s="13"/>

</xml_diff>

<commit_message>
Create and update functions added for users, sesssions and cookies added, scrum updated,
</commit_message>
<xml_diff>
--- a/ScrumProjectKesa.xlsx
+++ b/ScrumProjectKesa.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c0ec9f24d8d72cc2/OmatAsiat/GitHubRepos/ProjectKesa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="439" documentId="13_ncr:1_{EBFB5D00-5B16-4383-ADE2-85B692247430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C1612C6-4607-47D1-B43B-FCBA3C77ED8D}"/>
+  <xr:revisionPtr revIDLastSave="478" documentId="13_ncr:1_{EBFB5D00-5B16-4383-ADE2-85B692247430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0840EF40-BC71-4707-86C0-B2205CFF4EB1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="835" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,6 @@
     <sheet name="sprint_backlog_sprint3" sheetId="17" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="137">
   <si>
     <t>Content</t>
   </si>
@@ -415,6 +414,42 @@
   </si>
   <si>
     <t>Login servlet created uses post method</t>
+  </si>
+  <si>
+    <t>JS to refresh the page once update buttonis clicked or enter is pressed</t>
+  </si>
+  <si>
+    <t>rest service to update name that calls function from dao</t>
+  </si>
+  <si>
+    <t>rest service to update email that calls function from dao</t>
+  </si>
+  <si>
+    <t>rest service to update gender that calls function from dao</t>
+  </si>
+  <si>
+    <t>rest service to update birthdate that calls function from dao</t>
+  </si>
+  <si>
+    <t>User Story #4: As a user, I am able to delete my profile.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rest service to update Password that calls function from dao also hidden behind a password </t>
+  </si>
+  <si>
+    <t>As a user, I am able to login and logout.</t>
+  </si>
+  <si>
+    <t>servlets to login and out</t>
+  </si>
+  <si>
+    <t>User Story #2: As a user, I am able to login and logout.</t>
+  </si>
+  <si>
+    <t>logout servlet that invalidate sessions and redirects to login page</t>
+  </si>
+  <si>
+    <t>rest service to delete accout calss a function from dao</t>
   </si>
 </sst>
 </file>
@@ -900,7 +935,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1079,6 +1114,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3927,8 +3963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62CD205-9E86-46AF-9920-145C3DB823CA}">
   <dimension ref="C1:M64"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView showGridLines="0" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4220,26 +4256,26 @@
       <c r="D29" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="E29" s="16"/>
+      <c r="E29" s="84"/>
     </row>
     <row r="30" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C30" s="33"/>
       <c r="D30" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="E30" s="16"/>
+      <c r="E30" s="84"/>
     </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C31" s="33" t="s">
         <v>55</v>
       </c>
       <c r="D31" s="33"/>
-      <c r="E31" s="16"/>
+      <c r="E31" s="84"/>
     </row>
     <row r="32" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C32" s="33"/>
       <c r="D32" s="33"/>
-      <c r="E32" s="16"/>
+      <c r="E32" s="84"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C33" s="35"/>
@@ -4251,21 +4287,23 @@
       <c r="D34" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="E34" s="16"/>
+      <c r="E34" s="84"/>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C35" s="34" t="s">
-        <v>56</v>
+        <v>132</v>
       </c>
       <c r="D35" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="E35" s="16"/>
+      <c r="E35" s="84"/>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="16"/>
+      <c r="D36" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="E36" s="84"/>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C37" s="35"/>
@@ -4329,7 +4367,7 @@
       <c r="D46" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="E46" s="16"/>
+      <c r="E46" s="84"/>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C47" s="34" t="s">
@@ -4338,21 +4376,21 @@
       <c r="D47" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="E47" s="16"/>
+      <c r="E47" s="84"/>
     </row>
     <row r="48" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C48" s="34"/>
       <c r="D48" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="E48" s="16"/>
+      <c r="E48" s="84"/>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C49" s="34"/>
       <c r="D49" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="E49" s="16"/>
+      <c r="E49" s="84"/>
     </row>
     <row r="50" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C50" s="35"/>
@@ -4364,19 +4402,19 @@
       <c r="D51" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="E51" s="68"/>
+      <c r="E51" s="16"/>
     </row>
     <row r="52" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C52" s="32" t="s">
         <v>62</v>
       </c>
       <c r="D52" s="32"/>
-      <c r="E52" s="68"/>
+      <c r="E52" s="16"/>
     </row>
     <row r="53" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C53" s="32"/>
       <c r="D53" s="32"/>
-      <c r="E53" s="68"/>
+      <c r="E53" s="16"/>
     </row>
     <row r="54" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C54" s="35"/>
@@ -4412,31 +4450,31 @@
       <c r="D59" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="E59" s="68"/>
+      <c r="E59" s="16"/>
     </row>
     <row r="60" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C60" s="34"/>
       <c r="D60" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="E60" s="68"/>
+      <c r="E60" s="16"/>
     </row>
     <row r="61" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C61" s="34" t="s">
         <v>60</v>
       </c>
       <c r="D61" s="34"/>
-      <c r="E61" s="68"/>
+      <c r="E61" s="16"/>
     </row>
     <row r="62" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C62" s="34"/>
       <c r="D62" s="34"/>
-      <c r="E62" s="68"/>
+      <c r="E62" s="16"/>
     </row>
     <row r="63" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C63" s="34"/>
       <c r="D63" s="34"/>
-      <c r="E63" s="68"/>
+      <c r="E63" s="16"/>
     </row>
     <row r="64" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C64" s="35"/>
@@ -4643,7 +4681,7 @@
   <dimension ref="A1:S42"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5096,7 +5134,7 @@
       </c>
       <c r="C18" s="37"/>
       <c r="D18" s="37" t="s">
-        <v>102</v>
+        <v>42</v>
       </c>
       <c r="E18" s="46"/>
       <c r="F18" s="46"/>
@@ -5688,7 +5726,7 @@
   <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5761,13 +5799,15 @@
     </row>
     <row r="3" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>97</v>
+        <v>134</v>
       </c>
       <c r="B3" s="11">
         <v>6</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
+      <c r="D3" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
@@ -5790,7 +5830,9 @@
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
+      <c r="D4" s="47" t="s">
+        <v>42</v>
+      </c>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
@@ -5813,7 +5855,9 @@
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
+      <c r="D5" s="47" t="s">
+        <v>42</v>
+      </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
@@ -5836,7 +5880,9 @@
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
+      <c r="D6" s="47" t="s">
+        <v>42</v>
+      </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -5859,7 +5905,9 @@
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
+      <c r="D7" s="47" t="s">
+        <v>42</v>
+      </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
@@ -5881,7 +5929,9 @@
         <v>123</v>
       </c>
       <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
+      <c r="D8" s="47" t="s">
+        <v>42</v>
+      </c>
       <c r="I8" s="13"/>
       <c r="J8" s="14"/>
       <c r="K8" s="14"/>
@@ -5895,10 +5945,14 @@
       <c r="S8" s="14"/>
     </row>
     <row r="9" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="61"/>
+      <c r="A9" s="61" t="s">
+        <v>135</v>
+      </c>
       <c r="B9" s="13"/>
       <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
+      <c r="D9" s="47" t="s">
+        <v>42</v>
+      </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
@@ -6028,7 +6082,9 @@
         <v>4</v>
       </c>
       <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
+      <c r="D15" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
@@ -6046,10 +6102,14 @@
       <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
+      <c r="A16" s="13" t="s">
+        <v>126</v>
+      </c>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
+      <c r="D16" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
@@ -6067,10 +6127,14 @@
       <c r="S16" s="14"/>
     </row>
     <row r="17" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
+      <c r="A17" s="13" t="s">
+        <v>125</v>
+      </c>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
+      <c r="D17" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
@@ -6088,10 +6152,14 @@
       <c r="S17" s="14"/>
     </row>
     <row r="18" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
+      <c r="A18" s="13" t="s">
+        <v>127</v>
+      </c>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
+      <c r="D18" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
@@ -6109,10 +6177,14 @@
       <c r="S18" s="14"/>
     </row>
     <row r="19" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
+      <c r="A19" s="13" t="s">
+        <v>128</v>
+      </c>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
+      <c r="D19" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
@@ -6130,10 +6202,14 @@
       <c r="S19" s="14"/>
     </row>
     <row r="20" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
+      <c r="A20" s="13" t="s">
+        <v>129</v>
+      </c>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
+      <c r="D20" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
@@ -6151,10 +6227,14 @@
       <c r="S20" s="14"/>
     </row>
     <row r="21" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
+      <c r="A21" s="13" t="s">
+        <v>131</v>
+      </c>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
+      <c r="D21" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
@@ -6193,10 +6273,14 @@
       <c r="S22" s="14"/>
     </row>
     <row r="23" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
+      <c r="A23" s="11" t="s">
+        <v>130</v>
+      </c>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
+      <c r="D23" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
@@ -6214,10 +6298,14 @@
       <c r="S23" s="14"/>
     </row>
     <row r="24" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
+      <c r="A24" s="13" t="s">
+        <v>136</v>
+      </c>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
+      <c r="D24" s="13" t="s">
+        <v>76</v>
+      </c>
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>

</xml_diff>

<commit_message>
Profile deletion function. Scrum update. Other updates
</commit_message>
<xml_diff>
--- a/ScrumProjectKesa.xlsx
+++ b/ScrumProjectKesa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c0ec9f24d8d72cc2/OmatAsiat/GitHubRepos/ProjectKesa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="478" documentId="13_ncr:1_{EBFB5D00-5B16-4383-ADE2-85B692247430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0840EF40-BC71-4707-86C0-B2205CFF4EB1}"/>
+  <xr:revisionPtr revIDLastSave="500" documentId="13_ncr:1_{EBFB5D00-5B16-4383-ADE2-85B692247430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8215FCF-D928-4523-B1B3-66E5700C978E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="835" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="835" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guide" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="140">
   <si>
     <t>Content</t>
   </si>
@@ -188,9 +188,6 @@
     <t>DAY 5</t>
   </si>
   <si>
-    <t>Date: 25.4.2022</t>
-  </si>
-  <si>
     <t>SM Clone</t>
   </si>
   <si>
@@ -326,9 +323,6 @@
     <t xml:space="preserve">Connect to users db table and delete the profile basedon the ID </t>
   </si>
   <si>
-    <t xml:space="preserve">Sprint Backlog : Sprint 3 </t>
-  </si>
-  <si>
     <t xml:space="preserve">User Story #1:  As a user, I am able to register and become a registerd user. </t>
   </si>
   <si>
@@ -389,12 +383,6 @@
     <t>Create a doa function to check for duplicate emails and return an error message for the user</t>
   </si>
   <si>
-    <t>Sprint Backlog : Sprint 1 22.06.22- 03.08.22</t>
-  </si>
-  <si>
-    <t>Sprint Backlog : Sprint 2 03.08.22-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Create a function to show the a message once sign up is completed on main page. </t>
   </si>
   <si>
@@ -450,6 +438,27 @@
   </si>
   <si>
     <t>rest service to delete accout calss a function from dao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deletion confirmatio window </t>
+  </si>
+  <si>
+    <t>Return to login page after deletion by invalidating the session</t>
+  </si>
+  <si>
+    <t>Sprint Backlog : Sprint 1 22.06.22 - 03.08.22</t>
+  </si>
+  <si>
+    <t>Sprint Backlog : Sprint 2 03.08.22 - 19.08.22</t>
+  </si>
+  <si>
+    <t>Sprint Backlog : Sprint 3 19.08.22 -</t>
+  </si>
+  <si>
+    <t>Date: 19.08.2022</t>
+  </si>
+  <si>
+    <t>User Story #5: As a user, I am able to upload profile picture.</t>
   </si>
 </sst>
 </file>
@@ -1079,6 +1088,7 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1114,7 +1124,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3441,7 +3450,7 @@
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
       <c r="D2" s="31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E2" s="31"/>
       <c r="F2" s="31"/>
@@ -3450,7 +3459,7 @@
     </row>
     <row r="3" spans="2:8" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B3" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -3461,7 +3470,7 @@
     </row>
     <row r="4" spans="2:8" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B4" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -3471,13 +3480,13 @@
       <c r="H4" s="31"/>
     </row>
     <row r="6" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C6" s="71" t="s">
+      <c r="C6" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C7" s="29"/>
@@ -3551,12 +3560,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
     </row>
     <row r="2" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -3582,7 +3591,7 @@
     </row>
     <row r="4" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="2">
         <v>6</v>
@@ -3593,7 +3602,7 @@
     </row>
     <row r="5" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="2">
         <v>6</v>
@@ -3604,7 +3613,7 @@
     </row>
     <row r="6" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="2">
         <v>6</v>
@@ -3615,7 +3624,7 @@
     </row>
     <row r="7" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="2">
         <v>4</v>
@@ -3626,7 +3635,7 @@
     </row>
     <row r="8" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="2">
         <v>6</v>
@@ -3637,7 +3646,7 @@
     </row>
     <row r="9" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="2">
         <v>2</v>
@@ -3648,7 +3657,7 @@
     </row>
     <row r="10" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" s="2">
         <v>4</v>
@@ -3659,7 +3668,7 @@
     </row>
     <row r="11" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" s="2">
         <v>4</v>
@@ -3670,7 +3679,7 @@
     </row>
     <row r="12" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="2">
         <v>4</v>
@@ -3681,7 +3690,7 @@
     </row>
     <row r="13" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="2">
         <v>4</v>
@@ -3692,7 +3701,7 @@
     </row>
     <row r="14" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" s="2">
         <v>2</v>
@@ -3753,8 +3762,8 @@
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
-      <c r="F24" s="72"/>
-      <c r="G24" s="72"/>
+      <c r="F24" s="73"/>
+      <c r="G24" s="73"/>
     </row>
     <row r="25" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
@@ -3963,8 +3972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62CD205-9E86-46AF-9920-145C3DB823CA}">
   <dimension ref="C1:M64"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3975,14 +3984,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="76"/>
+      <c r="D1" s="77"/>
     </row>
     <row r="2" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
     </row>
     <row r="3" spans="3:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="C3" s="20" t="s">
@@ -3992,112 +4001,112 @@
         <v>17</v>
       </c>
       <c r="E3" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="78" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="77" t="s">
-        <v>74</v>
-      </c>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
-      <c r="M3" s="77"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="78"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="78"/>
     </row>
     <row r="4" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="32"/>
       <c r="D4" s="32"/>
-      <c r="E4" s="16"/>
-      <c r="H4" s="78" t="s">
+      <c r="E4" s="71"/>
+      <c r="H4" s="79" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="79" t="s">
-        <v>75</v>
-      </c>
-      <c r="L4" s="79"/>
-      <c r="M4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="80" t="s">
+        <v>74</v>
+      </c>
+      <c r="L4" s="80"/>
+      <c r="M4" s="80"/>
     </row>
     <row r="5" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="32"/>
       <c r="D5" s="32"/>
-      <c r="E5" s="16"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="79"/>
-      <c r="M5" s="79"/>
+      <c r="E5" s="71"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="80"/>
+      <c r="M5" s="80"/>
     </row>
     <row r="6" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6" s="32"/>
-      <c r="E6" s="16"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="79"/>
-      <c r="L6" s="79"/>
-      <c r="M6" s="79"/>
+      <c r="E6" s="71"/>
+      <c r="H6" s="79"/>
+      <c r="I6" s="79"/>
+      <c r="J6" s="79"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="80"/>
     </row>
     <row r="7" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="32"/>
       <c r="D7" s="32"/>
-      <c r="E7" s="16"/>
-      <c r="H7" s="78"/>
-      <c r="I7" s="78"/>
-      <c r="J7" s="78"/>
-      <c r="K7" s="79"/>
-      <c r="L7" s="79"/>
-      <c r="M7" s="79"/>
+      <c r="E7" s="71"/>
+      <c r="H7" s="79"/>
+      <c r="I7" s="79"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="80"/>
+      <c r="L7" s="80"/>
+      <c r="M7" s="80"/>
     </row>
     <row r="8" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="32"/>
       <c r="D8" s="32"/>
-      <c r="E8" s="16"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="78"/>
-      <c r="J8" s="78"/>
-      <c r="K8" s="79"/>
-      <c r="L8" s="79"/>
-      <c r="M8" s="79"/>
+      <c r="E8" s="71"/>
+      <c r="H8" s="79"/>
+      <c r="I8" s="79"/>
+      <c r="J8" s="79"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="80"/>
+      <c r="M8" s="80"/>
     </row>
     <row r="9" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="35"/>
       <c r="D9" s="35"/>
       <c r="E9" s="35"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="78"/>
-      <c r="J9" s="78"/>
-      <c r="K9" s="79"/>
-      <c r="L9" s="79"/>
-      <c r="M9" s="79"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="79"/>
+      <c r="J9" s="79"/>
+      <c r="K9" s="80"/>
+      <c r="L9" s="80"/>
+      <c r="M9" s="80"/>
     </row>
     <row r="10" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="33"/>
       <c r="D10" s="33"/>
       <c r="E10" s="69"/>
-      <c r="H10" s="78"/>
-      <c r="I10" s="78"/>
-      <c r="J10" s="78"/>
-      <c r="K10" s="79"/>
-      <c r="L10" s="79"/>
-      <c r="M10" s="79"/>
+      <c r="H10" s="79"/>
+      <c r="I10" s="79"/>
+      <c r="J10" s="79"/>
+      <c r="K10" s="80"/>
+      <c r="L10" s="80"/>
+      <c r="M10" s="80"/>
     </row>
     <row r="11" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="33"/>
       <c r="D11" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E11" s="69"/>
-      <c r="H11" s="78"/>
-      <c r="I11" s="78"/>
-      <c r="J11" s="78"/>
-      <c r="K11" s="79"/>
-      <c r="L11" s="79"/>
-      <c r="M11" s="79"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="79"/>
+      <c r="J11" s="79"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="80"/>
+      <c r="M11" s="80"/>
     </row>
     <row r="12" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="33" t="s">
@@ -4107,12 +4116,12 @@
         <v>18</v>
       </c>
       <c r="E12" s="69"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="78"/>
-      <c r="J12" s="78"/>
-      <c r="K12" s="79"/>
-      <c r="L12" s="79"/>
-      <c r="M12" s="79"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="79"/>
+      <c r="J12" s="79"/>
+      <c r="K12" s="80"/>
+      <c r="L12" s="80"/>
+      <c r="M12" s="80"/>
     </row>
     <row r="13" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="33"/>
@@ -4120,34 +4129,34 @@
         <v>19</v>
       </c>
       <c r="E13" s="69"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="78"/>
-      <c r="J13" s="78"/>
-      <c r="K13" s="79"/>
-      <c r="L13" s="79"/>
-      <c r="M13" s="79"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="79"/>
+      <c r="J13" s="79"/>
+      <c r="K13" s="80"/>
+      <c r="L13" s="80"/>
+      <c r="M13" s="80"/>
     </row>
     <row r="14" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="33"/>
       <c r="D14" s="33"/>
       <c r="E14" s="69"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="78"/>
-      <c r="J14" s="78"/>
-      <c r="K14" s="79"/>
-      <c r="L14" s="79"/>
-      <c r="M14" s="79"/>
+      <c r="H14" s="79"/>
+      <c r="I14" s="79"/>
+      <c r="J14" s="79"/>
+      <c r="K14" s="80"/>
+      <c r="L14" s="80"/>
+      <c r="M14" s="80"/>
     </row>
     <row r="15" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C15" s="35"/>
       <c r="D15" s="35"/>
       <c r="E15" s="35"/>
-      <c r="I15" s="74" t="s">
-        <v>76</v>
-      </c>
-      <c r="J15" s="75"/>
-      <c r="K15" s="75"/>
-      <c r="L15" s="75"/>
+      <c r="I15" s="75" t="s">
+        <v>75</v>
+      </c>
+      <c r="J15" s="76"/>
+      <c r="K15" s="76"/>
+      <c r="L15" s="76"/>
     </row>
     <row r="16" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C16" s="34"/>
@@ -4155,23 +4164,23 @@
         <v>20</v>
       </c>
       <c r="E16" s="68"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="75"/>
-      <c r="K16" s="75"/>
-      <c r="L16" s="75"/>
+      <c r="I16" s="76"/>
+      <c r="J16" s="76"/>
+      <c r="K16" s="76"/>
+      <c r="L16" s="76"/>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C17" s="34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D17" s="34" t="s">
         <v>21</v>
       </c>
       <c r="E17" s="68"/>
-      <c r="I17" s="75"/>
-      <c r="J17" s="75"/>
-      <c r="K17" s="75"/>
-      <c r="L17" s="75"/>
+      <c r="I17" s="76"/>
+      <c r="J17" s="76"/>
+      <c r="K17" s="76"/>
+      <c r="L17" s="76"/>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C18" s="34"/>
@@ -4179,19 +4188,19 @@
         <v>22</v>
       </c>
       <c r="E18" s="68"/>
-      <c r="I18" s="75"/>
-      <c r="J18" s="75"/>
-      <c r="K18" s="75"/>
-      <c r="L18" s="75"/>
+      <c r="I18" s="76"/>
+      <c r="J18" s="76"/>
+      <c r="K18" s="76"/>
+      <c r="L18" s="76"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C19" s="34"/>
       <c r="D19" s="34"/>
       <c r="E19" s="68"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="75"/>
-      <c r="K19" s="75"/>
-      <c r="L19" s="75"/>
+      <c r="I19" s="76"/>
+      <c r="J19" s="76"/>
+      <c r="K19" s="76"/>
+      <c r="L19" s="76"/>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C20" s="35"/>
@@ -4201,13 +4210,13 @@
     <row r="21" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C21" s="32"/>
       <c r="D21" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E21" s="68"/>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C22" s="32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D22" s="32" t="s">
         <v>23</v>
@@ -4228,13 +4237,13 @@
     <row r="25" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C25" s="34"/>
       <c r="D25" s="34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E25" s="68"/>
     </row>
     <row r="26" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C26" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D26" s="34" t="s">
         <v>23</v>
@@ -4254,28 +4263,28 @@
     <row r="29" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C29" s="33"/>
       <c r="D29" s="33" t="s">
-        <v>77</v>
-      </c>
-      <c r="E29" s="84"/>
+        <v>76</v>
+      </c>
+      <c r="E29" s="71"/>
     </row>
     <row r="30" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C30" s="33"/>
       <c r="D30" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" s="84"/>
+        <v>78</v>
+      </c>
+      <c r="E30" s="71"/>
     </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C31" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D31" s="33"/>
-      <c r="E31" s="84"/>
+      <c r="E31" s="71"/>
     </row>
     <row r="32" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C32" s="33"/>
       <c r="D32" s="33"/>
-      <c r="E32" s="84"/>
+      <c r="E32" s="71"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C33" s="35"/>
@@ -4285,25 +4294,25 @@
     <row r="34" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C34" s="34"/>
       <c r="D34" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="E34" s="84"/>
+        <v>71</v>
+      </c>
+      <c r="E34" s="71"/>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C35" s="34" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D35" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="E35" s="84"/>
+        <v>77</v>
+      </c>
+      <c r="E35" s="71"/>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C36" s="34"/>
       <c r="D36" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="E36" s="84"/>
+        <v>129</v>
+      </c>
+      <c r="E36" s="71"/>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C37" s="35"/>
@@ -4319,7 +4328,7 @@
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C39" s="32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D39" s="32"/>
       <c r="E39" s="68"/>
@@ -4337,23 +4346,23 @@
     <row r="42" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C42" s="33"/>
       <c r="D42" s="33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E42" s="68"/>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C43" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D43" s="33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E43" s="68"/>
     </row>
     <row r="44" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C44" s="33"/>
       <c r="D44" s="33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E44" s="68"/>
     </row>
@@ -4365,32 +4374,32 @@
     <row r="46" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C46" s="34"/>
       <c r="D46" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="E46" s="84"/>
+        <v>86</v>
+      </c>
+      <c r="E46" s="71"/>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C47" s="34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D47" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="E47" s="84"/>
+        <v>87</v>
+      </c>
+      <c r="E47" s="71"/>
     </row>
     <row r="48" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C48" s="34"/>
       <c r="D48" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="E48" s="84"/>
+        <v>89</v>
+      </c>
+      <c r="E48" s="71"/>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C49" s="34"/>
       <c r="D49" s="34" t="s">
-        <v>89</v>
-      </c>
-      <c r="E49" s="84"/>
+        <v>88</v>
+      </c>
+      <c r="E49" s="71"/>
     </row>
     <row r="50" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C50" s="35"/>
@@ -4400,13 +4409,13 @@
     <row r="51" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C51" s="32"/>
       <c r="D51" s="32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E51" s="16"/>
     </row>
     <row r="52" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C52" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D52" s="32"/>
       <c r="E52" s="16"/>
@@ -4424,13 +4433,13 @@
     <row r="55" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C55" s="33"/>
       <c r="D55" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E55" s="68"/>
     </row>
     <row r="56" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C56" s="33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D56" s="33"/>
       <c r="E56" s="68"/>
@@ -4448,33 +4457,33 @@
     <row r="59" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C59" s="34"/>
       <c r="D59" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="E59" s="16"/>
+        <v>92</v>
+      </c>
+      <c r="E59" s="71"/>
     </row>
     <row r="60" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C60" s="34"/>
       <c r="D60" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="E60" s="16"/>
+        <v>93</v>
+      </c>
+      <c r="E60" s="71"/>
     </row>
     <row r="61" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C61" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D61" s="34"/>
-      <c r="E61" s="16"/>
+      <c r="E61" s="71"/>
     </row>
     <row r="62" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C62" s="34"/>
       <c r="D62" s="34"/>
-      <c r="E62" s="16"/>
+      <c r="E62" s="71"/>
     </row>
     <row r="63" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C63" s="34"/>
       <c r="D63" s="34"/>
-      <c r="E63" s="16"/>
+      <c r="E63" s="71"/>
     </row>
     <row r="64" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C64" s="35"/>
@@ -4502,7 +4511,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4524,16 +4533,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="27" t="s">
         <v>64</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -4551,7 +4560,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -4559,7 +4568,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -4577,7 +4586,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4585,7 +4594,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -4595,13 +4604,15 @@
       <c r="A9" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>49</v>
+        <v>138</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -4609,7 +4620,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -4633,7 +4644,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -4681,7 +4692,7 @@
   <dimension ref="A1:S42"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection sqref="A1:S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4693,27 +4704,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="80" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
-      <c r="L1" s="81"/>
-      <c r="M1" s="81"/>
-      <c r="N1" s="81"/>
-      <c r="O1" s="81"/>
-      <c r="P1" s="81"/>
-      <c r="Q1" s="81"/>
-      <c r="R1" s="81"/>
-      <c r="S1" s="81"/>
+      <c r="A1" s="81" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="82"/>
+      <c r="S1" s="82"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
@@ -4781,7 +4792,7 @@
     </row>
     <row r="4" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="61" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B4" s="45"/>
       <c r="C4" s="36"/>
@@ -4806,7 +4817,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" s="37">
         <v>3</v>
@@ -4833,7 +4844,7 @@
     </row>
     <row r="6" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="60" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B6" s="48"/>
       <c r="C6" s="49"/>
@@ -4858,7 +4869,7 @@
     </row>
     <row r="7" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="60" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B7" s="48"/>
       <c r="C7" s="49"/>
@@ -4883,7 +4894,7 @@
     </row>
     <row r="8" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="60" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B8" s="47"/>
       <c r="C8" s="49"/>
@@ -4950,7 +4961,7 @@
     </row>
     <row r="11" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B11" s="37">
         <v>2</v>
@@ -4977,7 +4988,7 @@
     </row>
     <row r="12" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B12" s="47"/>
       <c r="C12" s="51"/>
@@ -5002,7 +5013,7 @@
     </row>
     <row r="13" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="47" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B13" s="47"/>
       <c r="C13" s="51"/>
@@ -5027,7 +5038,7 @@
     </row>
     <row r="14" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B14" s="47"/>
       <c r="C14" s="51"/>
@@ -5052,7 +5063,7 @@
     </row>
     <row r="15" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="47" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B15" s="47"/>
       <c r="C15" s="51"/>
@@ -5077,7 +5088,7 @@
     </row>
     <row r="16" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="47" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B16" s="47"/>
       <c r="C16" s="51"/>
@@ -5102,7 +5113,7 @@
     </row>
     <row r="17" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="58" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B17" s="47"/>
       <c r="C17" s="49"/>
@@ -5127,7 +5138,7 @@
     </row>
     <row r="18" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="50" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B18" s="37">
         <v>4</v>
@@ -5154,7 +5165,7 @@
     </row>
     <row r="19" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="60" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B19" s="47"/>
       <c r="C19" s="47"/>
@@ -5179,7 +5190,7 @@
     </row>
     <row r="20" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="60" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B20" s="47"/>
       <c r="C20" s="47"/>
@@ -5204,7 +5215,7 @@
     </row>
     <row r="21" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="60" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B21" s="47"/>
       <c r="C21" s="47"/>
@@ -5229,7 +5240,7 @@
     </row>
     <row r="22" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="58" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B22" s="47"/>
       <c r="C22" s="47"/>
@@ -5254,7 +5265,7 @@
     </row>
     <row r="23" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="58" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B23" s="47"/>
       <c r="C23" s="47"/>
@@ -5279,7 +5290,7 @@
     </row>
     <row r="24" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="58" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B24" s="47"/>
       <c r="C24" s="47"/>
@@ -5304,14 +5315,14 @@
     </row>
     <row r="25" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="50" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B25" s="37">
         <v>6</v>
       </c>
       <c r="C25" s="37"/>
       <c r="D25" s="37" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E25" s="46"/>
       <c r="F25" s="46"/>
@@ -5415,14 +5426,14 @@
     </row>
     <row r="30" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="37" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B30" s="37">
         <v>4</v>
       </c>
       <c r="C30" s="37"/>
       <c r="D30" s="37" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E30" s="46"/>
       <c r="F30" s="46"/>
@@ -5725,8 +5736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B586DF3-05CE-45CD-BBBF-F44EAB136942}">
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5736,27 +5747,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="82" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="83"/>
+      <c r="A1" s="83" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
     </row>
     <row r="2" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -5799,13 +5810,13 @@
     </row>
     <row r="3" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B3" s="11">
         <v>6</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="37" t="s">
         <v>42</v>
       </c>
       <c r="E3" s="12"/>
@@ -5826,7 +5837,7 @@
     </row>
     <row r="4" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="47"/>
@@ -5851,7 +5862,7 @@
     </row>
     <row r="5" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="63" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="47"/>
@@ -5876,7 +5887,7 @@
     </row>
     <row r="6" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="64" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="47"/>
@@ -5901,7 +5912,7 @@
     </row>
     <row r="7" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="63" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="47"/>
@@ -5926,7 +5937,7 @@
     </row>
     <row r="8" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="61" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C8" s="49"/>
       <c r="D8" s="47" t="s">
@@ -5946,7 +5957,7 @@
     </row>
     <row r="9" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="61" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="47"/>
@@ -6076,13 +6087,13 @@
     </row>
     <row r="15" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B15" s="11">
         <v>4</v>
       </c>
       <c r="C15" s="12"/>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="37" t="s">
         <v>42</v>
       </c>
       <c r="E15" s="12"/>
@@ -6103,7 +6114,7 @@
     </row>
     <row r="16" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
@@ -6128,7 +6139,7 @@
     </row>
     <row r="17" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
@@ -6153,7 +6164,7 @@
     </row>
     <row r="18" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -6178,7 +6189,7 @@
     </row>
     <row r="19" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
@@ -6203,7 +6214,7 @@
     </row>
     <row r="20" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
@@ -6228,7 +6239,7 @@
     </row>
     <row r="21" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
@@ -6274,12 +6285,14 @@
     </row>
     <row r="23" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="B23" s="11"/>
+        <v>126</v>
+      </c>
+      <c r="B23" s="11">
+        <v>2</v>
+      </c>
       <c r="C23" s="12"/>
-      <c r="D23" s="12" t="s">
-        <v>76</v>
+      <c r="D23" s="37" t="s">
+        <v>42</v>
       </c>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
@@ -6299,13 +6312,897 @@
     </row>
     <row r="24" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
       <c r="D24" s="13" t="s">
-        <v>76</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="14"/>
+      <c r="S24" s="14"/>
+    </row>
+    <row r="25" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
+      <c r="O25" s="14"/>
+      <c r="P25" s="14"/>
+      <c r="Q25" s="14"/>
+      <c r="R25" s="14"/>
+      <c r="S25" s="14"/>
+    </row>
+    <row r="26" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="14"/>
+      <c r="P26" s="14"/>
+      <c r="Q26" s="14"/>
+      <c r="R26" s="14"/>
+      <c r="S26" s="14"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="14"/>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="14"/>
+      <c r="S27" s="14"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14"/>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="14"/>
+      <c r="S28" s="14"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="14"/>
+      <c r="P29" s="14"/>
+      <c r="Q29" s="14"/>
+      <c r="R29" s="14"/>
+      <c r="S29" s="14"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="14"/>
+      <c r="P30" s="14"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="14"/>
+      <c r="S30" s="14"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="14"/>
+      <c r="P31" s="14"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="14"/>
+      <c r="S31" s="14"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="14"/>
+      <c r="P32" s="14"/>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="14"/>
+      <c r="S32" s="14"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="14"/>
+      <c r="S33" s="14"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="14"/>
+      <c r="P34" s="14"/>
+      <c r="Q34" s="14"/>
+      <c r="R34" s="14"/>
+      <c r="S34" s="14"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="14"/>
+      <c r="P35" s="14"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="14"/>
+      <c r="S35" s="14"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
+      <c r="S36" s="14"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37" s="13"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="14"/>
+      <c r="S38" s="14"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9">
+        <f>SUM(E4:E38)</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="9">
+        <f>SUM(F3:F38)</f>
+        <v>0</v>
+      </c>
+      <c r="G39" s="9">
+        <f>SUM(G3:G38)</f>
+        <v>0</v>
+      </c>
+      <c r="H39" s="9">
+        <f>SUM(H3:H38)</f>
+        <v>0</v>
+      </c>
+      <c r="I39" s="9">
+        <f>SUM(I3:I38)</f>
+        <v>0</v>
+      </c>
+      <c r="J39" s="14"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="14"/>
+      <c r="Q39" s="14"/>
+      <c r="R39" s="14"/>
+      <c r="S39" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:S1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{106689C9-A0BB-4B82-90C0-E17CAF16FC55}">
+  <dimension ref="A1:S39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="105.5" customWidth="1"/>
+    <col min="2" max="9" width="11.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="83" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+    </row>
+    <row r="2" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+    </row>
+    <row r="3" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+    </row>
+    <row r="4" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="66"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+    </row>
+    <row r="5" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="66"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+    </row>
+    <row r="6" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="66"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+    </row>
+    <row r="7" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="66"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+    </row>
+    <row r="8" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="66"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+    </row>
+    <row r="9" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="66"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+    </row>
+    <row r="10" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="66"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+    </row>
+    <row r="11" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="66"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+    </row>
+    <row r="12" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="66"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+    </row>
+    <row r="13" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+    </row>
+    <row r="14" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+    </row>
+    <row r="15" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+    </row>
+    <row r="16" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+    </row>
+    <row r="17" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="14"/>
+    </row>
+    <row r="18" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+    </row>
+    <row r="19" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
+    </row>
+    <row r="20" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+    </row>
+    <row r="21" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="14"/>
+    </row>
+    <row r="22" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
+    </row>
+    <row r="23" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
+    </row>
+    <row r="24" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
@@ -6661,876 +7558,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{106689C9-A0BB-4B82-90C0-E17CAF16FC55}">
-  <dimension ref="A1:S39"/>
-  <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:S1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="105.5" customWidth="1"/>
-    <col min="2" max="9" width="11.25" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="82" t="s">
-        <v>95</v>
-      </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="83"/>
-    </row>
-    <row r="2" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-    </row>
-    <row r="3" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-    </row>
-    <row r="4" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="66"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-    </row>
-    <row r="5" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="66"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-    </row>
-    <row r="6" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="66"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
-    </row>
-    <row r="7" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="66"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
-    </row>
-    <row r="8" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="66"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-    </row>
-    <row r="9" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="66"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
-    </row>
-    <row r="10" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="66"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14"/>
-    </row>
-    <row r="11" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="66"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
-    </row>
-    <row r="12" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="66"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
-    </row>
-    <row r="13" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
-    </row>
-    <row r="14" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-    </row>
-    <row r="15" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
-    </row>
-    <row r="16" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-    </row>
-    <row r="17" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
-    </row>
-    <row r="18" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="14"/>
-    </row>
-    <row r="19" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14"/>
-    </row>
-    <row r="20" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
-    </row>
-    <row r="21" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
-    </row>
-    <row r="22" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="14"/>
-    </row>
-    <row r="23" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="14"/>
-      <c r="S23" s="14"/>
-    </row>
-    <row r="24" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="14"/>
-    </row>
-    <row r="25" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="14"/>
-      <c r="Q25" s="14"/>
-      <c r="R25" s="14"/>
-      <c r="S25" s="14"/>
-    </row>
-    <row r="26" spans="1:19" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="14"/>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
-      <c r="Q29" s="14"/>
-      <c r="R29" s="14"/>
-      <c r="S29" s="14"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="14"/>
-      <c r="Q30" s="14"/>
-      <c r="R30" s="14"/>
-      <c r="S30" s="14"/>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
-      <c r="P31" s="14"/>
-      <c r="Q31" s="14"/>
-      <c r="R31" s="14"/>
-      <c r="S31" s="14"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="14"/>
-      <c r="Q32" s="14"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="14"/>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="14"/>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="14"/>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="14"/>
-      <c r="P34" s="14"/>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="14"/>
-      <c r="S34" s="14"/>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
-      <c r="P35" s="14"/>
-      <c r="Q35" s="14"/>
-      <c r="R35" s="14"/>
-      <c r="S35" s="14"/>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
-      <c r="P36" s="14"/>
-      <c r="Q36" s="14"/>
-      <c r="R36" s="14"/>
-      <c r="S36" s="14"/>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="14"/>
-      <c r="Q37" s="14"/>
-      <c r="R37" s="14"/>
-      <c r="S37" s="14"/>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
-      <c r="Q38" s="14"/>
-      <c r="R38" s="14"/>
-      <c r="S38" s="14"/>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9">
-        <f>SUM(E4:E38)</f>
-        <v>0</v>
-      </c>
-      <c r="F39" s="9">
-        <f>SUM(F3:F38)</f>
-        <v>0</v>
-      </c>
-      <c r="G39" s="9">
-        <f>SUM(G3:G38)</f>
-        <v>0</v>
-      </c>
-      <c r="H39" s="9">
-        <f>SUM(H3:H38)</f>
-        <v>0</v>
-      </c>
-      <c r="I39" s="9">
-        <f>SUM(I3:I38)</f>
-        <v>0</v>
-      </c>
-      <c r="J39" s="14"/>
-      <c r="K39" s="14"/>
-      <c r="L39" s="14"/>
-      <c r="M39" s="14"/>
-      <c r="N39" s="14"/>
-      <c r="O39" s="14"/>
-      <c r="P39" s="14"/>
-      <c r="Q39" s="14"/>
-      <c r="R39" s="14"/>
-      <c r="S39" s="14"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:S1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>